<commit_message>
the guarny e lobby 1 winner
</commit_message>
<xml_diff>
--- a/backend/lobby/lobbys.xlsx
+++ b/backend/lobby/lobbys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzoparenti/Desktop/Gran Turismo™ 7/github/worldtourbyTLM/backend/lobby/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C12BCD3-0A93-9047-B3E0-B52A4018F203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD8C775-29A3-C947-B4D7-D37C6E50C861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="960" windowWidth="27140" windowHeight="16440" xr2:uid="{A720D240-71C2-5742-B1A8-DCE80BADF5D1}"/>
   </bookViews>
@@ -1505,10 +1505,10 @@
             <v xml:space="preserve">Tlm-rupetheking </v>
           </cell>
           <cell r="F14" t="str">
-            <v>RMT _SILVERMAN-AC</v>
+            <v>Talsigiano</v>
           </cell>
           <cell r="G14" t="str">
-            <v>L.Silvestri</v>
+            <v xml:space="preserve">Talsigiano </v>
           </cell>
         </row>
         <row r="15">
@@ -1519,45 +1519,41 @@
             <v>M.Di Bartolo</v>
           </cell>
           <cell r="F15" t="str">
-            <v>Talsigiano</v>
+            <v>jack-187-jack</v>
           </cell>
           <cell r="G15" t="str">
-            <v xml:space="preserve">Talsigiano </v>
+            <v>Jack187</v>
           </cell>
         </row>
         <row r="16">
           <cell r="B16" t="str">
-            <v>TheGuarny</v>
+            <v>RMT _SILVERMAN-AC</v>
           </cell>
           <cell r="C16" t="str">
-            <v>TLM_TheGuarny</v>
+            <v>L.Silvestri</v>
           </cell>
           <cell r="F16" t="str">
-            <v>jack-187-jack</v>
+            <v>TLM_Verce90</v>
           </cell>
           <cell r="G16" t="str">
-            <v>Jack187</v>
+            <v>Verce</v>
           </cell>
         </row>
         <row r="17">
           <cell r="B17"/>
           <cell r="C17"/>
           <cell r="F17" t="str">
-            <v>TLM_Verce90</v>
+            <v>Mancinelli2002</v>
           </cell>
           <cell r="G17" t="str">
-            <v>Verce</v>
+            <v>Gian</v>
           </cell>
         </row>
         <row r="18">
           <cell r="B18"/>
           <cell r="C18"/>
-          <cell r="F18" t="str">
-            <v>Mancinelli2002</v>
-          </cell>
-          <cell r="G18" t="str">
-            <v>Gian</v>
-          </cell>
+          <cell r="F18"/>
+          <cell r="G18"/>
         </row>
         <row r="19">
           <cell r="B19"/>
@@ -1748,8 +1744,12 @@
           </cell>
         </row>
         <row r="40">
-          <cell r="B40"/>
-          <cell r="C40"/>
+          <cell r="B40" t="str">
+            <v>TheGuarny</v>
+          </cell>
+          <cell r="C40" t="str">
+            <v>TLM_TheGuarny</v>
+          </cell>
           <cell r="F40" t="str">
             <v>Blokkobubbles</v>
           </cell>
@@ -2280,15 +2280,15 @@
       </c>
       <c r="B12" s="2" t="str">
         <f>[1]LOBBY!B16</f>
-        <v>TheGuarny</v>
+        <v>RMT _SILVERMAN-AC</v>
       </c>
       <c r="C12" s="2" t="str">
         <f>[1]LOBBY!C16</f>
-        <v>TLM_TheGuarny</v>
+        <v>L.Silvestri</v>
       </c>
       <c r="D12" t="str">
         <f>IFERROR(VLOOKUP(B12,[1]nomi!$B:$G,6,FALSE),"")</f>
-        <v>TLM</v>
+        <v>RMT</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.2">
@@ -2513,15 +2513,15 @@
       </c>
       <c r="B10" s="2" t="str">
         <f>[1]LOBBY!F14</f>
-        <v>RMT _SILVERMAN-AC</v>
+        <v>Talsigiano</v>
       </c>
       <c r="C10" s="2" t="str">
         <f>[1]LOBBY!G14</f>
-        <v>L.Silvestri</v>
+        <v xml:space="preserve">Talsigiano </v>
       </c>
       <c r="D10" t="str">
         <f>IFERROR(VLOOKUP(B10,[1]nomi!$B:$G,6,FALSE),"")</f>
-        <v>RMT</v>
+        <v>TLMA</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="19" x14ac:dyDescent="0.2">
@@ -2530,11 +2530,11 @@
       </c>
       <c r="B11" s="2" t="str">
         <f>[1]LOBBY!F15</f>
-        <v>Talsigiano</v>
+        <v>jack-187-jack</v>
       </c>
       <c r="C11" s="2" t="str">
         <f>[1]LOBBY!G15</f>
-        <v xml:space="preserve">Talsigiano </v>
+        <v>Jack187</v>
       </c>
       <c r="D11" t="str">
         <f>IFERROR(VLOOKUP(B11,[1]nomi!$B:$G,6,FALSE),"")</f>
@@ -2547,15 +2547,15 @@
       </c>
       <c r="B12" s="2" t="str">
         <f>[1]LOBBY!F16</f>
-        <v>jack-187-jack</v>
+        <v>TLM_Verce90</v>
       </c>
       <c r="C12" s="2" t="str">
         <f>[1]LOBBY!G16</f>
-        <v>Jack187</v>
+        <v>Verce</v>
       </c>
       <c r="D12" t="str">
         <f>IFERROR(VLOOKUP(B12,[1]nomi!$B:$G,6,FALSE),"")</f>
-        <v>TLMA</v>
+        <v>TLM</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.2">
@@ -2564,32 +2564,32 @@
       </c>
       <c r="B13" s="2" t="str">
         <f>[1]LOBBY!F17</f>
-        <v>TLM_Verce90</v>
+        <v>Mancinelli2002</v>
       </c>
       <c r="C13" s="2" t="str">
         <f>[1]LOBBY!G17</f>
-        <v>Verce</v>
+        <v>Gian</v>
       </c>
       <c r="D13" t="str">
         <f>IFERROR(VLOOKUP(B13,[1]nomi!$B:$G,6,FALSE),"")</f>
-        <v>TLM</v>
+        <v>TLMA</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="str">
+      <c r="B14" s="2">
         <f>[1]LOBBY!F18</f>
-        <v>Mancinelli2002</v>
-      </c>
-      <c r="C14" s="2" t="str">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
         <f>[1]LOBBY!G18</f>
-        <v>Gian</v>
+        <v>0</v>
       </c>
       <c r="D14" t="str">
         <f>IFERROR(VLOOKUP(B14,[1]nomi!$B:$G,6,FALSE),"")</f>
-        <v>TLMA</v>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:4" ht="19" x14ac:dyDescent="0.2">
@@ -2863,17 +2863,17 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="2" t="str">
         <f>[1]LOBBY!B40</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="2">
+        <v>TheGuarny</v>
+      </c>
+      <c r="C15" s="2" t="str">
         <f>[1]LOBBY!C40</f>
-        <v>0</v>
+        <v>TLM_TheGuarny</v>
       </c>
       <c r="D15" t="str">
         <f>IFERROR(VLOOKUP(B15,[1]nomi!$B:$G,6,FALSE),"")</f>
-        <v/>
+        <v>TLM</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mod varie flag numeri
</commit_message>
<xml_diff>
--- a/backend/lobby/lobbys.xlsx
+++ b/backend/lobby/lobbys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzoparenti/Desktop/Gran Turismo™ 7/github/finoalconfineTLM/backend/lobby/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A539591E-494C-C543-806A-B03382C1CDBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70A8C96-8ED1-574F-8E22-B7CC0758130B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="960" windowWidth="27140" windowHeight="16440" xr2:uid="{A720D240-71C2-5742-B1A8-DCE80BADF5D1}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>n</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>team</t>
+  </si>
+  <si>
+    <t>naz</t>
   </si>
 </sst>
 </file>
@@ -181,6 +184,9 @@
           <cell r="G1" t="str">
             <v>sigla</v>
           </cell>
+          <cell r="H1" t="str">
+            <v>naz</v>
+          </cell>
         </row>
         <row r="2">
           <cell r="B2" t="str">
@@ -201,6 +207,9 @@
           <cell r="G2" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H2" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="3">
           <cell r="B3" t="str">
@@ -221,6 +230,9 @@
           <cell r="G3" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H3" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="4">
           <cell r="B4" t="str">
@@ -241,6 +253,9 @@
           <cell r="G4" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H4" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="5">
           <cell r="B5" t="str">
@@ -261,6 +276,9 @@
           <cell r="G5" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H5" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="6">
           <cell r="B6" t="str">
@@ -281,6 +299,9 @@
           <cell r="G6" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H6" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="7">
           <cell r="B7" t="str">
@@ -301,6 +322,9 @@
           <cell r="G7" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H7" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="8">
           <cell r="B8" t="str">
@@ -321,6 +345,9 @@
           <cell r="G8" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H8" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="9">
           <cell r="B9" t="str">
@@ -341,6 +368,9 @@
           <cell r="G9" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H9" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="10">
           <cell r="B10" t="str">
@@ -361,6 +391,9 @@
           <cell r="G10" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H10" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="11">
           <cell r="B11" t="str">
@@ -381,6 +414,9 @@
           <cell r="G11" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H11" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="12">
           <cell r="B12" t="str">
@@ -401,6 +437,9 @@
           <cell r="G12" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H12" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="13">
           <cell r="B13" t="str">
@@ -421,6 +460,9 @@
           <cell r="G13" t="str">
             <v>GTRC</v>
           </cell>
+          <cell r="H13" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="14">
           <cell r="B14" t="str">
@@ -441,6 +483,9 @@
           <cell r="G14" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H14" t="str">
+            <v>de</v>
+          </cell>
         </row>
         <row r="15">
           <cell r="B15" t="str">
@@ -461,6 +506,9 @@
           <cell r="G15" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H15" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="16">
           <cell r="B16" t="str">
@@ -481,6 +529,9 @@
           <cell r="G16" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H16" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="17">
           <cell r="B17" t="str">
@@ -501,6 +552,9 @@
           <cell r="G17" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H17" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="18">
           <cell r="B18" t="str">
@@ -521,6 +575,9 @@
           <cell r="G18" t="str">
             <v>TLMA</v>
           </cell>
+          <cell r="H18" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="19">
           <cell r="B19" t="str">
@@ -541,6 +598,9 @@
           <cell r="G19" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H19" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="20">
           <cell r="B20" t="str">
@@ -561,6 +621,9 @@
           <cell r="G20" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H20" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="21">
           <cell r="B21" t="str">
@@ -581,6 +644,9 @@
           <cell r="G21" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H21" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="22">
           <cell r="B22" t="str">
@@ -601,6 +667,9 @@
           <cell r="G22" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H22" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="23">
           <cell r="B23" t="str">
@@ -621,6 +690,9 @@
           <cell r="G23" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H23" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="24">
           <cell r="B24" t="str">
@@ -641,6 +713,9 @@
           <cell r="G24" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H24" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="25">
           <cell r="B25" t="str">
@@ -661,6 +736,9 @@
           <cell r="G25" t="str">
             <v>DRT</v>
           </cell>
+          <cell r="H25" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="26">
           <cell r="B26" t="str">
@@ -681,6 +759,9 @@
           <cell r="G26" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H26" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="27">
           <cell r="B27" t="str">
@@ -701,6 +782,9 @@
           <cell r="G27" t="str">
             <v>GTRC</v>
           </cell>
+          <cell r="H27" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="28">
           <cell r="B28" t="str">
@@ -721,6 +805,9 @@
           <cell r="G28" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H28" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="29">
           <cell r="B29" t="str">
@@ -741,6 +828,9 @@
           <cell r="G29" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H29" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="30">
           <cell r="B30" t="str">
@@ -761,6 +851,9 @@
           <cell r="G30" t="str">
             <v>GTRC</v>
           </cell>
+          <cell r="H30" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="31">
           <cell r="B31" t="str">
@@ -781,6 +874,9 @@
           <cell r="G31" t="str">
             <v>RMT</v>
           </cell>
+          <cell r="H31" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="32">
           <cell r="B32" t="str">
@@ -801,6 +897,9 @@
           <cell r="G32" t="str">
             <v>RMT</v>
           </cell>
+          <cell r="H32" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="33">
           <cell r="B33" t="str">
@@ -821,6 +920,9 @@
           <cell r="G33" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H33" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="34">
           <cell r="B34" t="str">
@@ -841,6 +943,9 @@
           <cell r="G34" t="str">
             <v>RMT</v>
           </cell>
+          <cell r="H34" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="35">
           <cell r="B35" t="str">
@@ -861,6 +966,9 @@
           <cell r="G35" t="str">
             <v>GTRC</v>
           </cell>
+          <cell r="H35" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="36">
           <cell r="B36" t="str">
@@ -881,6 +989,9 @@
           <cell r="G36" t="str">
             <v>TLMA</v>
           </cell>
+          <cell r="H36" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="37">
           <cell r="B37" t="str">
@@ -901,6 +1012,9 @@
           <cell r="G37" t="str">
             <v>TLMA</v>
           </cell>
+          <cell r="H37" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="38">
           <cell r="B38" t="str">
@@ -921,6 +1035,9 @@
           <cell r="G38" t="str">
             <v>RMT</v>
           </cell>
+          <cell r="H38" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="39">
           <cell r="B39" t="str">
@@ -941,6 +1058,9 @@
           <cell r="G39" t="str">
             <v>TLMA</v>
           </cell>
+          <cell r="H39" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="40">
           <cell r="B40" t="str">
@@ -961,6 +1081,9 @@
           <cell r="G40" t="str">
             <v>TLMA</v>
           </cell>
+          <cell r="H40" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="41">
           <cell r="B41" t="str">
@@ -981,6 +1104,9 @@
           <cell r="G41" t="str">
             <v>RMT</v>
           </cell>
+          <cell r="H41" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="42">
           <cell r="B42" t="str">
@@ -1001,6 +1127,9 @@
           <cell r="G42" t="str">
             <v>GTRC</v>
           </cell>
+          <cell r="H42" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="43">
           <cell r="B43" t="str">
@@ -1021,6 +1150,9 @@
           <cell r="G43" t="str">
             <v>CSC</v>
           </cell>
+          <cell r="H43" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="44">
           <cell r="B44" t="str">
@@ -1041,6 +1173,9 @@
           <cell r="G44" t="str">
             <v>GTRC</v>
           </cell>
+          <cell r="H44" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="45">
           <cell r="B45" t="str">
@@ -1061,6 +1196,9 @@
           <cell r="G45" t="str">
             <v>TLMA</v>
           </cell>
+          <cell r="H45" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="46">
           <cell r="B46" t="str">
@@ -1081,6 +1219,9 @@
           <cell r="G46" t="str">
             <v>TLMA</v>
           </cell>
+          <cell r="H46" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="47">
           <cell r="B47" t="str">
@@ -1101,6 +1242,9 @@
           <cell r="G47" t="str">
             <v>GTRC</v>
           </cell>
+          <cell r="H47" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="48">
           <cell r="B48" t="str">
@@ -1121,6 +1265,9 @@
           <cell r="G48" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H48" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="49">
           <cell r="B49" t="str">
@@ -1141,6 +1288,9 @@
           <cell r="G49" t="str">
             <v>GTRC</v>
           </cell>
+          <cell r="H49" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="50">
           <cell r="B50" t="str">
@@ -1161,6 +1311,9 @@
           <cell r="G50" t="str">
             <v>CSC</v>
           </cell>
+          <cell r="H50" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="51">
           <cell r="B51" t="str">
@@ -1181,6 +1334,9 @@
           <cell r="G51" t="str">
             <v>DCT</v>
           </cell>
+          <cell r="H51" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="52">
           <cell r="B52" t="str">
@@ -1201,6 +1357,9 @@
           <cell r="G52" t="str">
             <v>DCT</v>
           </cell>
+          <cell r="H52" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="53">
           <cell r="B53" t="str">
@@ -1221,6 +1380,9 @@
           <cell r="G53" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H53" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="54">
           <cell r="B54" t="str">
@@ -1241,6 +1403,9 @@
           <cell r="G54" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H54" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="55">
           <cell r="B55" t="str">
@@ -1261,6 +1426,9 @@
           <cell r="G55" t="str">
             <v>GTID</v>
           </cell>
+          <cell r="H55" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="56">
           <cell r="B56" t="str">
@@ -1281,6 +1449,9 @@
           <cell r="G56" t="str">
             <v>GTID</v>
           </cell>
+          <cell r="H56" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="57">
           <cell r="B57" t="str">
@@ -1301,6 +1472,9 @@
           <cell r="G57" t="str">
             <v>GTID</v>
           </cell>
+          <cell r="H57" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="58">
           <cell r="B58" t="str">
@@ -1312,6 +1486,9 @@
           <cell r="G58" t="str">
             <v>DCT</v>
           </cell>
+          <cell r="H58" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="59">
           <cell r="B59" t="str">
@@ -1323,6 +1500,9 @@
           <cell r="G59" t="str">
             <v>BAD</v>
           </cell>
+          <cell r="H59" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="60">
           <cell r="B60" t="str">
@@ -1334,6 +1514,9 @@
           <cell r="G60" t="str">
             <v>DRT</v>
           </cell>
+          <cell r="H60" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="61">
           <cell r="B61" t="str">
@@ -1345,6 +1528,9 @@
           <cell r="G61" t="str">
             <v>RMT</v>
           </cell>
+          <cell r="H61" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="62">
           <cell r="B62" t="str">
@@ -1356,6 +1542,9 @@
           <cell r="G62" t="str">
             <v>TLMA</v>
           </cell>
+          <cell r="H62" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="63">
           <cell r="B63" t="str">
@@ -1367,33 +1556,42 @@
           <cell r="G63" t="str">
             <v>TLMA</v>
           </cell>
+          <cell r="H63" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="64">
           <cell r="B64" t="str">
             <v>Verce90</v>
           </cell>
           <cell r="C64" t="str">
-            <v>TLM Verce</v>
+            <v>TLM Verce90</v>
           </cell>
           <cell r="D64" t="str">
             <v>Team Lion Motorsport</v>
           </cell>
           <cell r="G64" t="str">
             <v>TLM</v>
+          </cell>
+          <cell r="H64" t="str">
+            <v>it</v>
           </cell>
         </row>
         <row r="65">
           <cell r="B65" t="str">
-            <v>Ulix90</v>
+            <v>Ulix1990</v>
           </cell>
           <cell r="C65" t="str">
-            <v>TLM_Ulix90</v>
+            <v>TLM_Ulix1990</v>
           </cell>
           <cell r="D65" t="str">
             <v>Team Lion Motorsport</v>
           </cell>
           <cell r="G65" t="str">
             <v>TLM</v>
+          </cell>
+          <cell r="H65" t="str">
+            <v>it</v>
           </cell>
         </row>
         <row r="66">
@@ -1409,19 +1607,25 @@
           <cell r="G66" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H66" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="67">
           <cell r="B67" t="str">
             <v>CTR_ocior-78</v>
           </cell>
           <cell r="C67" t="str">
-            <v>TLM_Ocior-78</v>
+            <v>TLM-Ocior78</v>
           </cell>
           <cell r="D67" t="str">
             <v>Team Lion Motorsport</v>
           </cell>
           <cell r="G67" t="str">
             <v>TLM</v>
+          </cell>
+          <cell r="H67" t="str">
+            <v>it</v>
           </cell>
         </row>
         <row r="68">
@@ -1431,6 +1635,9 @@
           <cell r="G68" t="str">
             <v>TLM</v>
           </cell>
+          <cell r="H68" t="str">
+            <v>it</v>
+          </cell>
         </row>
         <row r="69">
           <cell r="D69" t="str">
@@ -1438,6 +1645,9 @@
           </cell>
           <cell r="G69" t="str">
             <v>TLM</v>
+          </cell>
+          <cell r="H69" t="str">
+            <v>it</v>
           </cell>
         </row>
       </sheetData>
@@ -1561,7 +1771,7 @@
             <v>Verce90</v>
           </cell>
           <cell r="C14" t="str">
-            <v>TLM Verce</v>
+            <v>TLM Verce90</v>
           </cell>
           <cell r="F14" t="str">
             <v>TLM_michaelFox12</v>
@@ -1609,18 +1819,18 @@
             <v>Verce90</v>
           </cell>
           <cell r="G17" t="str">
-            <v>TLM Verce</v>
+            <v>TLM Verce90</v>
           </cell>
         </row>
         <row r="18">
           <cell r="B18" t="str">
-            <v>Ulix90</v>
+            <v>Ulix1990</v>
           </cell>
           <cell r="C18" t="str">
             <v>TLM_Ulix90</v>
           </cell>
           <cell r="F18" t="str">
-            <v>Ulix90</v>
+            <v>Ulix1990</v>
           </cell>
           <cell r="G18" t="str">
             <v>TLM_Ulix90</v>
@@ -1993,15 +2203,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE91598-8C93-844B-A02C-EA327E1FA7D6}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2014,10 +2224,13 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>[1]LOBBY!B6</f>
@@ -2031,10 +2244,14 @@
         <f>IFERROR(VLOOKUP(B2,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E2" t="str">
+        <f>IFERROR(VLOOKUP(B2,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>[1]LOBBY!B7</f>
@@ -2048,10 +2265,14 @@
         <f>IFERROR(VLOOKUP(B3,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E3" t="str">
+        <f>IFERROR(VLOOKUP(B3,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="B4" s="2" t="str">
         <f>[1]LOBBY!B8</f>
@@ -2065,10 +2286,14 @@
         <f>IFERROR(VLOOKUP(B4,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E4" t="str">
+        <f>IFERROR(VLOOKUP(B4,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="B5" s="2" t="str">
         <f>[1]LOBBY!B9</f>
@@ -2082,10 +2307,14 @@
         <f>IFERROR(VLOOKUP(B5,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E5" t="str">
+        <f>IFERROR(VLOOKUP(B5,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="B6" s="2" t="str">
         <f>[1]LOBBY!B10</f>
@@ -2099,10 +2328,14 @@
         <f>IFERROR(VLOOKUP(B6,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E6" t="str">
+        <f>IFERROR(VLOOKUP(B6,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>92</v>
       </c>
       <c r="B7" s="2" t="str">
         <f>[1]LOBBY!B11</f>
@@ -2116,10 +2349,14 @@
         <f>IFERROR(VLOOKUP(B7,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E7" t="str">
+        <f>IFERROR(VLOOKUP(B7,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="str">
         <f>[1]LOBBY!B12</f>
@@ -2133,10 +2370,14 @@
         <f>IFERROR(VLOOKUP(B8,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E8" t="str">
+        <f>IFERROR(VLOOKUP(B8,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="B9" s="2" t="str">
         <f>[1]LOBBY!B13</f>
@@ -2150,10 +2391,14 @@
         <f>IFERROR(VLOOKUP(B9,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E9" t="str">
+        <f>IFERROR(VLOOKUP(B9,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="str">
         <f>[1]LOBBY!B14</f>
@@ -2161,16 +2406,20 @@
       </c>
       <c r="C10" s="2" t="str">
         <f>[1]LOBBY!C14</f>
-        <v>TLM Verce</v>
+        <v>TLM Verce90</v>
       </c>
       <c r="D10" t="str">
         <f>IFERROR(VLOOKUP(B10,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E10" t="str">
+        <f>IFERROR(VLOOKUP(B10,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="B11" s="2" t="str">
         <f>[1]LOBBY!B15</f>
@@ -2184,10 +2433,14 @@
         <f>IFERROR(VLOOKUP(B11,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E11" t="str">
+        <f>IFERROR(VLOOKUP(B11,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="str">
         <f>[1]LOBBY!B16</f>
@@ -2201,10 +2454,14 @@
         <f>IFERROR(VLOOKUP(B12,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E12" t="str">
+        <f>IFERROR(VLOOKUP(B12,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="B13" s="2" t="str">
         <f>[1]LOBBY!B17</f>
@@ -2218,14 +2475,18 @@
         <f>IFERROR(VLOOKUP(B13,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E13" t="str">
+        <f>IFERROR(VLOOKUP(B13,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="str">
         <f>[1]LOBBY!B18</f>
-        <v>Ulix90</v>
+        <v>Ulix1990</v>
       </c>
       <c r="C14" s="2" t="str">
         <f>[1]LOBBY!C18</f>
@@ -2235,10 +2496,14 @@
         <f>IFERROR(VLOOKUP(B14,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E14" t="str">
+        <f>IFERROR(VLOOKUP(B14,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="str">
         <f>[1]LOBBY!B19</f>
@@ -2252,10 +2517,14 @@
         <f>IFERROR(VLOOKUP(B15,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E15" t="str">
+        <f>IFERROR(VLOOKUP(B15,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="B16" s="2" t="str">
         <f>[1]LOBBY!B20</f>
@@ -2269,10 +2538,14 @@
         <f>IFERROR(VLOOKUP(B16,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E16" t="str">
+        <f>IFERROR(VLOOKUP(B16,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="B17" s="2" t="str">
         <f>[1]LOBBY!B21</f>
@@ -2285,6 +2558,10 @@
       <c r="D17" t="str">
         <f>IFERROR(VLOOKUP(B17,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
+      </c>
+      <c r="E17" t="str">
+        <f>IFERROR(VLOOKUP(B17,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
       </c>
     </row>
   </sheetData>
@@ -2294,15 +2571,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7025A9D3-BB9F-C548-A2C6-B2B8CE175CE9}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2315,10 +2592,13 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="str">
         <f>[1]LOBBY!F6</f>
@@ -2332,10 +2612,14 @@
         <f>IFERROR(VLOOKUP(B2,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E2" t="str">
+        <f>IFERROR(VLOOKUP(B2,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="str">
         <f>[1]LOBBY!F7</f>
@@ -2349,10 +2633,14 @@
         <f>IFERROR(VLOOKUP(B3,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E3" t="str">
+        <f>IFERROR(VLOOKUP(B3,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="str">
         <f>[1]LOBBY!F8</f>
@@ -2366,10 +2654,14 @@
         <f>IFERROR(VLOOKUP(B4,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E4" t="str">
+        <f>IFERROR(VLOOKUP(B4,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="str">
         <f>[1]LOBBY!F9</f>
@@ -2383,10 +2675,14 @@
         <f>IFERROR(VLOOKUP(B5,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E5" t="str">
+        <f>IFERROR(VLOOKUP(B5,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B6" s="2" t="str">
         <f>[1]LOBBY!F10</f>
@@ -2400,10 +2696,14 @@
         <f>IFERROR(VLOOKUP(B6,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E6" t="str">
+        <f>IFERROR(VLOOKUP(B6,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="str">
         <f>[1]LOBBY!F11</f>
@@ -2417,10 +2717,14 @@
         <f>IFERROR(VLOOKUP(B7,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E7" t="str">
+        <f>IFERROR(VLOOKUP(B7,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>de</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="B8" s="2" t="str">
         <f>[1]LOBBY!F12</f>
@@ -2434,10 +2738,14 @@
         <f>IFERROR(VLOOKUP(B8,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E8" t="str">
+        <f>IFERROR(VLOOKUP(B8,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="str">
         <f>[1]LOBBY!F13</f>
@@ -2451,10 +2759,14 @@
         <f>IFERROR(VLOOKUP(B9,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E9" t="str">
+        <f>IFERROR(VLOOKUP(B9,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="str">
         <f>[1]LOBBY!F14</f>
@@ -2468,10 +2780,14 @@
         <f>IFERROR(VLOOKUP(B10,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E10" t="str">
+        <f>IFERROR(VLOOKUP(B10,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="B11" s="2" t="str">
         <f>[1]LOBBY!F15</f>
@@ -2485,10 +2801,14 @@
         <f>IFERROR(VLOOKUP(B11,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E11" t="str">
+        <f>IFERROR(VLOOKUP(B11,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B12" s="2" t="str">
         <f>[1]LOBBY!F16</f>
@@ -2502,10 +2822,14 @@
         <f>IFERROR(VLOOKUP(B12,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E12" t="str">
+        <f>IFERROR(VLOOKUP(B12,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B13" s="2" t="str">
         <f>[1]LOBBY!F17</f>
@@ -2513,20 +2837,24 @@
       </c>
       <c r="C13" s="2" t="str">
         <f>[1]LOBBY!G17</f>
-        <v>TLM Verce</v>
+        <v>TLM Verce90</v>
       </c>
       <c r="D13" t="str">
         <f>IFERROR(VLOOKUP(B13,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E13" t="str">
+        <f>IFERROR(VLOOKUP(B13,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="str">
         <f>[1]LOBBY!F18</f>
-        <v>Ulix90</v>
+        <v>Ulix1990</v>
       </c>
       <c r="C14" s="2" t="str">
         <f>[1]LOBBY!G18</f>
@@ -2536,10 +2864,14 @@
         <f>IFERROR(VLOOKUP(B14,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E14" t="str">
+        <f>IFERROR(VLOOKUP(B14,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="B15" s="2" t="str">
         <f>[1]LOBBY!F19</f>
@@ -2553,10 +2885,14 @@
         <f>IFERROR(VLOOKUP(B15,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E15" t="str">
+        <f>IFERROR(VLOOKUP(B15,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B16" s="2" t="str">
         <f>[1]LOBBY!F20</f>
@@ -2570,10 +2906,14 @@
         <f>IFERROR(VLOOKUP(B16,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+      <c r="E16" t="str">
+        <f>IFERROR(VLOOKUP(B16,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B17" s="2" t="str">
         <f>[1]LOBBY!F21</f>
@@ -2586,6 +2926,10 @@
       <c r="D17" t="str">
         <f>IFERROR(VLOOKUP(B17,[1]nomi!$B:$G,6,FALSE),"")</f>
         <v>TLM</v>
+      </c>
+      <c r="E17" t="str">
+        <f>IFERROR(VLOOKUP(B17,[1]nomi!$B:$H,7,FALSE),"")</f>
+        <v>it</v>
       </c>
     </row>
   </sheetData>

</xml_diff>